<commit_message>
trying again to save updated court example source doc
</commit_message>
<xml_diff>
--- a/docassemble/mlhframework/data/sources/court_sample.xlsx
+++ b/docassemble/mlhframework/data/sources/court_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmilyKressMiller\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9DED83-8893-4B03-BD5D-C236FE483411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE836853-65F6-4F68-A4FF-578308EF212C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1985,12 +1985,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2273,7 +2272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
@@ -5467,10 +5466,10 @@
       <c r="I89" t="s">
         <v>379</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="J89" t="s">
         <v>628</v>
       </c>
-      <c r="K89" s="2" t="s">
+      <c r="K89" t="s">
         <v>635</v>
       </c>
       <c r="L89" t="s">
@@ -5505,7 +5504,7 @@
       <c r="J90" t="s">
         <v>630</v>
       </c>
-      <c r="K90" s="2" t="s">
+      <c r="K90" t="s">
         <v>484</v>
       </c>
       <c r="L90" t="s">
@@ -5537,7 +5536,7 @@
       <c r="I91" t="s">
         <v>616</v>
       </c>
-      <c r="K91" s="2" t="s">
+      <c r="K91" t="s">
         <v>636</v>
       </c>
       <c r="L91" t="s">
@@ -5569,7 +5568,7 @@
       <c r="I92" t="s">
         <v>617</v>
       </c>
-      <c r="K92" s="2" t="s">
+      <c r="K92" t="s">
         <v>486</v>
       </c>
       <c r="L92" t="s">
@@ -5601,7 +5600,7 @@
       <c r="I93" t="s">
         <v>383</v>
       </c>
-      <c r="K93" s="2" t="s">
+      <c r="K93" t="s">
         <v>487</v>
       </c>
       <c r="L93" t="s">
@@ -5636,7 +5635,7 @@
       <c r="J94" t="s">
         <v>631</v>
       </c>
-      <c r="K94" s="2" t="s">
+      <c r="K94" t="s">
         <v>637</v>
       </c>
       <c r="L94" t="s">
@@ -5668,7 +5667,7 @@
       <c r="I95" t="s">
         <v>618</v>
       </c>
-      <c r="K95" s="2" t="s">
+      <c r="K95" t="s">
         <v>638</v>
       </c>
       <c r="L95" t="s">
@@ -5700,7 +5699,7 @@
       <c r="I96" t="s">
         <v>385</v>
       </c>
-      <c r="K96" s="2" t="s">
+      <c r="K96" t="s">
         <v>93</v>
       </c>
       <c r="L96" t="s">
@@ -5732,7 +5731,7 @@
       <c r="I97" t="s">
         <v>386</v>
       </c>
-      <c r="K97" s="2" t="s">
+      <c r="K97" t="s">
         <v>489</v>
       </c>
       <c r="L97" t="s">
@@ -5764,7 +5763,7 @@
       <c r="I98" t="s">
         <v>387</v>
       </c>
-      <c r="K98" s="2" t="s">
+      <c r="K98" t="s">
         <v>490</v>
       </c>
       <c r="L98" t="s">
@@ -5796,7 +5795,7 @@
       <c r="I99" t="s">
         <v>388</v>
       </c>
-      <c r="K99" s="2" t="s">
+      <c r="K99" t="s">
         <v>480</v>
       </c>
       <c r="L99" t="s">
@@ -5828,7 +5827,7 @@
       <c r="I100" t="s">
         <v>619</v>
       </c>
-      <c r="K100" s="2" t="s">
+      <c r="K100" t="s">
         <v>30</v>
       </c>
       <c r="L100" t="s">
@@ -5863,7 +5862,7 @@
       <c r="J101" t="s">
         <v>633</v>
       </c>
-      <c r="K101" s="2" t="s">
+      <c r="K101" t="s">
         <v>31</v>
       </c>
       <c r="L101" t="s">
@@ -5895,7 +5894,7 @@
       <c r="I102" t="s">
         <v>620</v>
       </c>
-      <c r="K102" s="2" t="s">
+      <c r="K102" t="s">
         <v>491</v>
       </c>
       <c r="L102" t="s">
@@ -5927,7 +5926,7 @@
       <c r="I103" t="s">
         <v>621</v>
       </c>
-      <c r="K103" s="2" t="s">
+      <c r="K103" t="s">
         <v>492</v>
       </c>
       <c r="L103" t="s">
@@ -5959,7 +5958,7 @@
       <c r="I104" t="s">
         <v>622</v>
       </c>
-      <c r="K104" s="2" t="s">
+      <c r="K104" t="s">
         <v>493</v>
       </c>
       <c r="L104" t="s">
@@ -5991,7 +5990,7 @@
       <c r="I105" t="s">
         <v>394</v>
       </c>
-      <c r="K105" s="2" t="s">
+      <c r="K105" t="s">
         <v>494</v>
       </c>
       <c r="L105" t="s">
@@ -6023,7 +6022,7 @@
       <c r="I106" t="s">
         <v>395</v>
       </c>
-      <c r="K106" s="2" t="s">
+      <c r="K106" t="s">
         <v>495</v>
       </c>
       <c r="L106" t="s">
@@ -6058,7 +6057,7 @@
       <c r="J107" t="s">
         <v>634</v>
       </c>
-      <c r="K107" s="2" t="s">
+      <c r="K107" t="s">
         <v>496</v>
       </c>
       <c r="L107" t="s">
@@ -6090,7 +6089,7 @@
       <c r="I108" t="s">
         <v>397</v>
       </c>
-      <c r="K108" s="2" t="s">
+      <c r="K108" t="s">
         <v>497</v>
       </c>
       <c r="L108" t="s">
@@ -6122,7 +6121,7 @@
       <c r="I109" t="s">
         <v>623</v>
       </c>
-      <c r="K109" s="2" t="s">
+      <c r="K109" t="s">
         <v>498</v>
       </c>
       <c r="L109" t="s">
@@ -6154,7 +6153,7 @@
       <c r="I110" t="s">
         <v>624</v>
       </c>
-      <c r="K110" s="2" t="s">
+      <c r="K110" t="s">
         <v>499</v>
       </c>
       <c r="L110" t="s">
@@ -6186,7 +6185,7 @@
       <c r="I111" t="s">
         <v>625</v>
       </c>
-      <c r="K111" s="2" t="s">
+      <c r="K111" t="s">
         <v>639</v>
       </c>
       <c r="L111" t="s">
@@ -6218,7 +6217,7 @@
       <c r="I112" t="s">
         <v>626</v>
       </c>
-      <c r="K112" s="2" t="s">
+      <c r="K112" t="s">
         <v>640</v>
       </c>
       <c r="L112" t="s">

</xml_diff>

<commit_message>
court info pull now working (updated python module), wrote questions,
</commit_message>
<xml_diff>
--- a/docassemble/mlhframework/data/sources/court_sample.xlsx
+++ b/docassemble/mlhframework/data/sources/court_sample.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmilyKressMiller\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE836853-65F6-4F68-A4FF-578308EF212C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6EBDE6-D3E9-41C5-BEA3-69C9F1594723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="640">
   <si>
     <t>name</t>
   </si>
@@ -326,9 +337,6 @@
     <t>Wexford</t>
   </si>
   <si>
-    <t>county</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -1937,9 +1945,6 @@
     <t>Bellainre</t>
   </si>
   <si>
-    <t>L&amp;apo;Anse</t>
-  </si>
-  <si>
     <t>Belulah</t>
   </si>
   <si>
@@ -1950,6 +1955,9 @@
   </si>
   <si>
     <t>Burton</t>
+  </si>
+  <si>
+    <t>address_county</t>
   </si>
 </sst>
 </file>
@@ -2272,13 +2280,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
     <col min="5" max="5" width="21.26953125" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
     <col min="8" max="8" width="22.90625" customWidth="1"/>
@@ -2294,16 +2302,16 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>639</v>
+      </c>
+      <c r="B1" t="s">
         <v>99</v>
       </c>
-      <c r="B1" t="s">
-        <v>100</v>
-      </c>
       <c r="C1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -2315,7 +2323,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -2350,31 +2358,31 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" t="s">
         <v>218</v>
       </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" t="s">
-        <v>219</v>
-      </c>
       <c r="H2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M2">
         <v>48740</v>
@@ -2397,28 +2405,28 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M3">
         <v>49862</v>
@@ -2432,31 +2440,31 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M4">
         <v>49010</v>
@@ -2470,31 +2478,31 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M5">
         <v>49707</v>
@@ -2505,34 +2513,34 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M6">
         <v>49615</v>
@@ -2543,31 +2551,31 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K7" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M7">
         <v>48658</v>
@@ -2578,31 +2586,31 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M8">
         <v>49946</v>
@@ -2613,31 +2621,31 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M9">
         <v>49058</v>
@@ -2648,28 +2656,28 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M10">
         <v>48708</v>
@@ -2680,28 +2688,28 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="L11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M11">
         <v>49617</v>
@@ -2712,31 +2720,31 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K12" t="s">
         <v>93</v>
       </c>
       <c r="L12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M12">
         <v>49085</v>
@@ -2747,31 +2755,31 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K13" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M13">
         <v>49036</v>
@@ -2782,31 +2790,31 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M14">
         <v>49014</v>
@@ -2817,31 +2825,31 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M15">
         <v>49031</v>
@@ -2852,31 +2860,31 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K16" t="s">
         <v>30</v>
       </c>
       <c r="L16" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M16">
         <v>49720</v>
@@ -2887,34 +2895,34 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K17" t="s">
         <v>31</v>
       </c>
       <c r="L17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M17">
         <v>49721</v>
@@ -2925,31 +2933,31 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K18" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M18">
         <v>49783</v>
@@ -2960,31 +2968,31 @@
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I19" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K19" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M19">
         <v>48625</v>
@@ -2995,34 +3003,34 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M20">
         <v>48879</v>
@@ -3033,31 +3041,31 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M21">
         <v>49738</v>
@@ -3068,31 +3076,31 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K22" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L22" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M22">
         <v>49829</v>
@@ -3103,34 +3111,34 @@
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I23" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J23" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K23" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L23" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M23">
         <v>49801</v>
@@ -3141,31 +3149,31 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I24" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K24" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L24" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M24">
         <v>48813</v>
@@ -3176,31 +3184,31 @@
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L25" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M25">
         <v>49770</v>
@@ -3211,31 +3219,31 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I26" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K26" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L26" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M26">
         <v>48502</v>
@@ -3246,31 +3254,31 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K27" t="s">
         <v>41</v>
       </c>
       <c r="L27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M27">
         <v>48624</v>
@@ -3281,34 +3289,34 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I28" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="L28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M28">
         <v>49911</v>
@@ -3319,31 +3327,31 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M29">
         <v>49684</v>
@@ -3354,34 +3362,34 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J30" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K30" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L30" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M30">
         <v>48847</v>
@@ -3392,31 +3400,31 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K31" t="s">
         <v>45</v>
       </c>
       <c r="L31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M31">
         <v>49242</v>
@@ -3427,31 +3435,31 @@
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I32" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K32" t="s">
         <v>46</v>
       </c>
       <c r="L32" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M32">
         <v>49931</v>
@@ -3462,31 +3470,31 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I33" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K33" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L33" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M33">
         <v>48413</v>
@@ -3497,34 +3505,34 @@
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I34" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J34" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K34" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L34" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M34">
         <v>48901</v>
@@ -3535,31 +3543,31 @@
         <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K35" t="s">
         <v>49</v>
       </c>
       <c r="L35" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M35">
         <v>48846</v>
@@ -3570,37 +3578,37 @@
         <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F36" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H36" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J36" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K36" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L36" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M36">
         <v>48764</v>
@@ -3611,31 +3619,31 @@
         <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L37" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M37">
         <v>49920</v>
@@ -3646,31 +3654,31 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H38" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I38" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K38" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L38" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M38">
         <v>48858</v>
@@ -3681,31 +3689,31 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I39" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K39" t="s">
         <v>53</v>
       </c>
       <c r="L39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M39">
         <v>49201</v>
@@ -3716,31 +3724,31 @@
         <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I40" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K40" t="s">
         <v>54</v>
       </c>
       <c r="L40" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M40">
         <v>49048</v>
@@ -3751,34 +3759,34 @@
         <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I41" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J41" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K41" t="s">
         <v>55</v>
       </c>
       <c r="L41" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M41">
         <v>49646</v>
@@ -3789,31 +3797,31 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H42" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I42" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K42" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L42" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M42">
         <v>49503</v>
@@ -3824,31 +3832,31 @@
         <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H43" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I43" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K43" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L43" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M43">
         <v>49950</v>
@@ -3859,31 +3867,31 @@
         <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I44" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J44" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K44" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M44">
         <v>49304</v>
@@ -3894,31 +3902,31 @@
         <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I45" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K45" t="s">
         <v>59</v>
       </c>
       <c r="L45" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M45">
         <v>48446</v>
@@ -3929,31 +3937,31 @@
         <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I46" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J46" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K46" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L46" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M46">
         <v>49682</v>
@@ -3964,31 +3972,31 @@
         <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H47" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I47" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K47" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L47" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M47">
         <v>49221</v>
@@ -3999,31 +4007,31 @@
         <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F48" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J48" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K48" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L48" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M48">
         <v>48843</v>
@@ -4034,31 +4042,31 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H49" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I49" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K49" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L49" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M49">
         <v>49868</v>
@@ -4069,31 +4077,31 @@
         <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H50" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I50" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K50" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L50" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M50">
         <v>49781</v>
@@ -4104,31 +4112,31 @@
         <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F51" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H51" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I51" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K51" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L51" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M51">
         <v>48043</v>
@@ -4139,31 +4147,31 @@
         <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I52" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J52" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K52" t="s">
         <v>66</v>
       </c>
       <c r="L52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M52">
         <v>49660</v>
@@ -4174,34 +4182,34 @@
         <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F53" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H53" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I53" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K53" t="s">
         <v>67</v>
       </c>
       <c r="L53" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M53">
         <v>49855</v>
@@ -4212,31 +4220,31 @@
         <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F54" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H54" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I54" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K54" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L54" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M54">
         <v>49431</v>
@@ -4247,31 +4255,31 @@
         <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F55" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I55" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K55" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L55" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M55">
         <v>49307</v>
@@ -4282,31 +4290,31 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F56" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H56" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I56" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K56" t="s">
         <v>70</v>
       </c>
       <c r="L56" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M56">
         <v>49858</v>
@@ -4317,31 +4325,31 @@
         <v>71</v>
       </c>
       <c r="B57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E57" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F57" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I57" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K57" t="s">
         <v>71</v>
       </c>
       <c r="L57" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M57">
         <v>48640</v>
@@ -4352,34 +4360,34 @@
         <v>72</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F58" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H58" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I58" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J58" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K58" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L58" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M58">
         <v>49651</v>
@@ -4390,31 +4398,31 @@
         <v>73</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E59" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F59" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H59" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I59" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K59" t="s">
         <v>73</v>
       </c>
       <c r="L59" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M59">
         <v>48161</v>
@@ -4425,34 +4433,34 @@
         <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F60" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H60" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I60" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J60" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K60" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L60" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M60">
         <v>48888</v>
@@ -4463,34 +4471,34 @@
         <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E61" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F61" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H61" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I61" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J61" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K61" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L61" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M61">
         <v>49709</v>
@@ -4501,31 +4509,31 @@
         <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D62" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E62" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F62" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H62" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I62" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K62" t="s">
         <v>76</v>
       </c>
       <c r="L62" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M62">
         <v>49442</v>
@@ -4536,37 +4544,37 @@
         <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F63" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H63" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I63" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J63" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K63" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L63" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M63">
         <v>49349</v>
@@ -4577,31 +4585,31 @@
         <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H64" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K64" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M64">
         <v>48341</v>
@@ -4612,34 +4620,34 @@
         <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E65" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F65" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I65" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J65" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K65" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L65" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M65">
         <v>49420</v>
@@ -4650,31 +4658,31 @@
         <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F66" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H66" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I66" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K66" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L66" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M66">
         <v>48661</v>
@@ -4685,31 +4693,31 @@
         <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C67" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E67" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F67" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H67" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I67" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K67" t="s">
         <v>81</v>
       </c>
       <c r="L67" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M67">
         <v>49953</v>
@@ -4720,31 +4728,31 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F68" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H68" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I68" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K68" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L68" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M68">
         <v>49677</v>
@@ -4755,31 +4763,31 @@
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C69" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D69" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F69" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H69" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I69" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K69" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L69" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M69">
         <v>48647</v>
@@ -4790,28 +4798,28 @@
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C70" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F70" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I70" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K70" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L70" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M70">
         <v>49735</v>
@@ -4822,31 +4830,31 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F71" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H71" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I71" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L71" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M71">
         <v>49417</v>
@@ -4857,31 +4865,31 @@
         <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E72" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F72" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I72" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J72" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K72" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L72" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M72">
         <v>49779</v>
@@ -4892,31 +4900,31 @@
         <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F73" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H73" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I73" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K73" t="s">
         <v>87</v>
       </c>
       <c r="L73" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M73">
         <v>48653</v>
@@ -4927,31 +4935,31 @@
         <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C74" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E74" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F74" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I74" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K74" t="s">
         <v>88</v>
       </c>
       <c r="L74" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M74">
         <v>48602</v>
@@ -4962,34 +4970,34 @@
         <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E75" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F75" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H75" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I75" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J75" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K75" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L75" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M75">
         <v>48471</v>
@@ -5000,34 +5008,34 @@
         <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F76" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H76" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I76" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J76" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K76" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L76" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M76">
         <v>49854</v>
@@ -5038,28 +5046,28 @@
         <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F77" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I77" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K77" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L77" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M77">
         <v>48817</v>
@@ -5070,31 +5078,31 @@
         <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E78" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F78" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H78" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I78" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K78" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L78" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M78">
         <v>48060</v>
@@ -5105,34 +5113,34 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C79" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F79" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H79" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I79" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J79" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K79" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L79" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M79">
         <v>49032</v>
@@ -5143,31 +5151,31 @@
         <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E80" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F80" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H80" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I80" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K80" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L80" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M80">
         <v>48723</v>
@@ -5178,31 +5186,31 @@
         <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D81" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F81" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H81" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I81" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K81" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L81" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M81">
         <v>49079</v>
@@ -5213,31 +5221,31 @@
         <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D82" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E82" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F82" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I82" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K82" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L82" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M82">
         <v>48107</v>
@@ -5248,31 +5256,31 @@
         <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C83" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D83" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F83" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H83" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I83" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K83" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L83" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M83">
         <v>48226</v>
@@ -5283,31 +5291,31 @@
         <v>98</v>
       </c>
       <c r="B84" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C84" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D84" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F84" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H84" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I84" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K84" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L84" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M84">
         <v>49601</v>
@@ -5318,31 +5326,31 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
+        <v>540</v>
+      </c>
+      <c r="C85" t="s">
+        <v>217</v>
+      </c>
+      <c r="D85" t="s">
         <v>541</v>
       </c>
-      <c r="C85" t="s">
-        <v>218</v>
-      </c>
-      <c r="D85" t="s">
-        <v>542</v>
-      </c>
       <c r="E85" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F85" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I85" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J85" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="K85" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L85" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M85">
         <v>48740</v>
@@ -5353,28 +5361,28 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C86" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D86" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E86" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F86" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I86" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K86" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L86" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M86">
         <v>49862</v>
@@ -5385,28 +5393,28 @@
         <v>18</v>
       </c>
       <c r="B87" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D87" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E87" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F87" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I87" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K87" t="s">
         <v>18</v>
       </c>
       <c r="L87" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M87">
         <v>49010</v>
@@ -5417,28 +5425,28 @@
         <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C88" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D88" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F88" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I88" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K88" t="s">
         <v>19</v>
       </c>
       <c r="L88" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M88">
         <v>49707</v>
@@ -5449,31 +5457,31 @@
         <v>20</v>
       </c>
       <c r="B89" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C89" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D89" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E89" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F89" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I89" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J89" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K89" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="L89" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M89">
         <v>49615</v>
@@ -5484,31 +5492,31 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
+        <v>540</v>
+      </c>
+      <c r="C90" t="s">
+        <v>217</v>
+      </c>
+      <c r="D90" t="s">
         <v>541</v>
       </c>
-      <c r="C90" t="s">
-        <v>218</v>
-      </c>
-      <c r="D90" t="s">
-        <v>542</v>
-      </c>
       <c r="E90" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F90" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I90" t="s">
+        <v>628</v>
+      </c>
+      <c r="J90" t="s">
         <v>629</v>
       </c>
-      <c r="J90" t="s">
-        <v>630</v>
-      </c>
       <c r="K90" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L90" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M90">
         <v>44444</v>
@@ -5519,28 +5527,28 @@
         <v>22</v>
       </c>
       <c r="B91" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C91" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D91" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E91" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F91" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I91" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K91" t="s">
-        <v>636</v>
+        <v>484</v>
       </c>
       <c r="L91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M91">
         <v>44444</v>
@@ -5551,28 +5559,28 @@
         <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C92" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D92" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E92" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F92" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I92" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K92" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L92" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M92">
         <v>44444</v>
@@ -5583,28 +5591,28 @@
         <v>24</v>
       </c>
       <c r="B93" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C93" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D93" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E93" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F93" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I93" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K93" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L93" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M93">
         <v>44444</v>
@@ -5615,31 +5623,31 @@
         <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D94" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E94" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F94" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I94" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J94" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="K94" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="L94" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M94">
         <v>44444</v>
@@ -5650,28 +5658,28 @@
         <v>26</v>
       </c>
       <c r="B95" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D95" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E95" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F95" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I95" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K95" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="L95" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M95">
         <v>44444</v>
@@ -5682,28 +5690,28 @@
         <v>26</v>
       </c>
       <c r="B96" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C96" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E96" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F96" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I96" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K96" t="s">
         <v>93</v>
       </c>
       <c r="L96" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M96">
         <v>44444</v>
@@ -5714,28 +5722,28 @@
         <v>27</v>
       </c>
       <c r="B97" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C97" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D97" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E97" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F97" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I97" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K97" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L97" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M97">
         <v>44444</v>
@@ -5746,28 +5754,28 @@
         <v>28</v>
       </c>
       <c r="B98" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C98" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D98" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E98" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F98" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I98" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K98" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L98" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M98">
         <v>44444</v>
@@ -5778,28 +5786,28 @@
         <v>29</v>
       </c>
       <c r="B99" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C99" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D99" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E99" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F99" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I99" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K99" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L99" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M99">
         <v>44444</v>
@@ -5810,28 +5818,28 @@
         <v>30</v>
       </c>
       <c r="B100" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C100" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D100" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E100" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F100" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I100" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K100" t="s">
         <v>30</v>
       </c>
       <c r="L100" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M100">
         <v>44444</v>
@@ -5842,31 +5850,31 @@
         <v>31</v>
       </c>
       <c r="B101" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D101" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E101" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F101" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I101" t="s">
+        <v>631</v>
+      </c>
+      <c r="J101" t="s">
         <v>632</v>
-      </c>
-      <c r="J101" t="s">
-        <v>633</v>
       </c>
       <c r="K101" t="s">
         <v>31</v>
       </c>
       <c r="L101" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M101">
         <v>44444</v>
@@ -5877,28 +5885,28 @@
         <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C102" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D102" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E102" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F102" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I102" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K102" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L102" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M102">
         <v>44444</v>
@@ -5909,28 +5917,28 @@
         <v>33</v>
       </c>
       <c r="B103" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C103" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D103" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E103" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F103" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I103" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K103" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L103" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M103">
         <v>44444</v>
@@ -5941,28 +5949,28 @@
         <v>34</v>
       </c>
       <c r="B104" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D104" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E104" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F104" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I104" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K104" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L104" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M104">
         <v>44444</v>
@@ -5973,28 +5981,28 @@
         <v>35</v>
       </c>
       <c r="B105" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C105" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D105" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E105" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F105" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I105" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K105" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L105" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M105">
         <v>44444</v>
@@ -6005,28 +6013,28 @@
         <v>36</v>
       </c>
       <c r="B106" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C106" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D106" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E106" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F106" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I106" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K106" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L106" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M106">
         <v>44444</v>
@@ -6037,31 +6045,31 @@
         <v>37</v>
       </c>
       <c r="B107" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D107" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E107" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F107" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I107" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J107" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="K107" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L107" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M107">
         <v>44444</v>
@@ -6072,28 +6080,28 @@
         <v>38</v>
       </c>
       <c r="B108" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C108" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D108" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E108" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F108" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I108" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K108" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L108" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M108">
         <v>44444</v>
@@ -6104,28 +6112,28 @@
         <v>39</v>
       </c>
       <c r="B109" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C109" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D109" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E109" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F109" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I109" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K109" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L109" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M109">
         <v>44444</v>
@@ -6136,28 +6144,28 @@
         <v>40</v>
       </c>
       <c r="B110" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C110" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D110" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E110" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F110" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I110" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="K110" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L110" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M110">
         <v>44444</v>
@@ -6168,28 +6176,28 @@
         <v>40</v>
       </c>
       <c r="B111" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C111" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D111" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E111" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F111" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I111" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="K111" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="L111" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M111">
         <v>44444</v>
@@ -6200,28 +6208,28 @@
         <v>40</v>
       </c>
       <c r="B112" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C112" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D112" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E112" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F112" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I112" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="K112" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="L112" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M112">
         <v>44444</v>

</xml_diff>